<commit_message>
Add support for importing from csv files
</commit_message>
<xml_diff>
--- a/lib/storage_import_template.xlsx
+++ b/lib/storage_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoiv\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoiv\Google Drive (khoivan88@aggienetwork.com)\From Khoi personal computer\Documents\Learning\open_eventory\open_enventory-developed-by-Khoi\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385ACA25-1FF1-413E-BEF5-3D417E64ADE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8122EC37-F476-4310-8D37-685C18083722}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" activeTab="1" xr2:uid="{3B9E381E-B69E-4854-B768-0EA51965DCF7}"/>
+    <workbookView xWindow="1395" yWindow="810" windowWidth="22605" windowHeight="12090" activeTab="1" xr2:uid="{3B9E381E-B69E-4854-B768-0EA51965DCF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Fill out this form" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>2. "Storage name" column is required, "storage barcode" can be left empty</t>
-  </si>
-  <si>
-    <t>4. Save as the excel file (only the "Fill out this form" sheet)  as "tab-delimited text file"</t>
   </si>
   <si>
     <t>5. Use the text file to import into Open Enventory data</t>
@@ -110,6 +107,9 @@
       </rPr>
       <t>Settings</t>
     </r>
+  </si>
+  <si>
+    <t>4. Save as the excel file (only the "Fill out this form" sheet)  as "Text (tab-delimited) (*.txt)" or "CSV (comma-delimited) (*.csv)"</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832464B3-C945-4F85-A69C-2941DAD880B3}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -560,17 +562,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for Excel files in Import and Delete; Fix bug for delete multiple chemicals function;
</commit_message>
<xml_diff>
--- a/lib/storage_import_template.xlsx
+++ b/lib/storage_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoiv\Google Drive (khoivan88@aggienetwork.com)\From Khoi personal computer\Documents\Learning\open_eventory\open_enventory-developed-by-Khoi\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8122EC37-F476-4310-8D37-685C18083722}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F841DC-7AA0-4E85-9750-F1D335B3E456}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="810" windowWidth="22605" windowHeight="12090" activeTab="1" xr2:uid="{3B9E381E-B69E-4854-B768-0EA51965DCF7}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="22605" windowHeight="12090" activeTab="1" xr2:uid="{3B9E381E-B69E-4854-B768-0EA51965DCF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Fill out this form" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Instruction:</t>
   </si>
@@ -109,7 +110,16 @@
     </r>
   </si>
   <si>
-    <t>4. Save as the excel file (only the "Fill out this form" sheet)  as "Text (tab-delimited) (*.txt)" or "CSV (comma-delimited) (*.csv)"</t>
+    <t>- "Text (tab-delimited) (*.txt)"</t>
+  </si>
+  <si>
+    <t>- "CSV (comma-delimited) (*.csv)"</t>
+  </si>
+  <si>
+    <t>- Excel files (*.xlsx and *.xls)</t>
+  </si>
+  <si>
+    <t>4. Save as the excel file (only the "Fill out this form" sheet) as any of the followings:</t>
   </si>
 </sst>
 </file>
@@ -174,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -186,6 +196,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -532,15 +543,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832464B3-C945-4F85-A69C-2941DAD880B3}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="138.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -565,13 +576,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>